<commit_message>
Added test spec for tag model class and tag model class
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Time Spent</t>
+    <t xml:space="preserve">Time Spent (manhours)</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -49,31 +49,79 @@
     <t xml:space="preserve">Persona </t>
   </si>
   <si>
+    <t xml:space="preserve">Who is the app for?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Working Weeks </t>
   </si>
   <si>
     <t xml:space="preserve">User Journey</t>
   </si>
   <si>
+    <t xml:space="preserve">What do they want to do ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hours per week</t>
   </si>
   <si>
+    <t xml:space="preserve">A3 Mapping/Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basically a tidy up of class notes &amp; train palaver</t>
+  </si>
+  <si>
     <t xml:space="preserve">Est Hourly Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitise Plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renaming app, applying notes to readme file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating file structure, setting up git and committing along the way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create DB, Create Schema, Create Seed data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merchant – CRUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created test spec and merchant model class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag – CRUD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,12 +181,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,16 +215,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J6"/>
+  <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -194,13 +255,13 @@
       <c r="I2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>43502</v>
+      <c r="A3" s="2" t="n">
+        <v>43503</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -211,15 +272,22 @@
       <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">B3*$J$6</f>
+        <v>29</v>
+      </c>
       <c r="I3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>43503</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -229,17 +297,24 @@
         <v>7</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <f aca="false">B4*$J$6</f>
+        <v>29</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>37.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>43503</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -248,17 +323,134 @@
       <c r="C5" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <f aca="false">B5*$J$6</f>
+        <v>29</v>
+      </c>
       <c r="I5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <f aca="false">J2/J3/J4</f>
         <v>14.4927536231884</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="0" t="n">
+      <c r="A6" s="3" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">B6*$J$6</f>
         <v>14.5</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <f aca="false">B7*$J$6</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">B8*$J$6</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">B9*$J$6</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>43504</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transaction spec and transaction model class - confrimed functional
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -100,10 +100,13 @@
     <t xml:space="preserve">Merchant – CRUD</t>
   </si>
   <si>
-    <t xml:space="preserve">Created test spec and merchant model class</t>
+    <t xml:space="preserve">Created merchant test spec and merchant model class</t>
   </si>
   <si>
     <t xml:space="preserve">Tag – CRUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created tag test spec and tag model class</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -442,7 +445,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Created main controller, layout and corresponding index for test
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,17 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Time Spent (manhours)</t>
+    <t xml:space="preserve">Manhours</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Iteration</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feature</t>
   </si>
   <si>
@@ -94,6 +97,9 @@
     <t xml:space="preserve">Create DB, Create Schema, Create Seed data</t>
   </si>
   <si>
+    <t xml:space="preserve">Total Hours</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implementation</t>
   </si>
   <si>
@@ -103,10 +109,25 @@
     <t xml:space="preserve">Created merchant test spec and merchant model class</t>
   </si>
   <si>
+    <t xml:space="preserve">Total Cost</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tag – CRUD</t>
   </si>
   <si>
     <t xml:space="preserve">Created tag test spec and tag model class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transactions – CRUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created transaction test spec and transaction model class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wireframing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before proceeding with views draw up wireframe using fixed model classes</t>
   </si>
 </sst>
 </file>
@@ -119,7 +140,7 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +161,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,17 +212,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -218,242 +262,313 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J11"/>
+  <dimension ref="A2:K12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="4" t="n">
         <v>43503</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <f aca="false">B3*$J$6</f>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <f aca="false">B3*$K$6</f>
         <v>29</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="4" t="n">
         <v>43503</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">B4*$J$6</f>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">B4*$K$6</f>
         <v>29</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3" t="n">
         <v>37.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="4" t="n">
         <v>43503</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">B5*$J$6</f>
+      <c r="F5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <f aca="false">B5*$K$6</f>
         <v>29</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <f aca="false">J2/J3/J4</f>
+      <c r="J5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <f aca="false">K2/K3/K4</f>
         <v>14.4927536231884</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>43504</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="A6" s="6" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <f aca="false">B6*$J$6</f>
+      <c r="F6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <f aca="false">B6*$K$6</f>
         <v>14.5</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="K6" s="3" t="n">
         <v>14.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>43504</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="A7" s="6" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <f aca="false">B7*$J$6</f>
+      <c r="F7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">B7*$K$6</f>
         <v>14.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>43504</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="A8" s="6" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">B8*$J$6</f>
+      <c r="F8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <f aca="false">B8*$K$6</f>
         <v>14.5</v>
       </c>
+      <c r="J8" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>43504</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="A9" s="6" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <f aca="false">B9*$J$6</f>
+      <c r="D9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <f aca="false">B9*$K$6</f>
         <v>14.5</v>
       </c>
+      <c r="J9" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>43504</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="6" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B10" s="5" t="n">
         <v>0.25</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>28</v>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <f aca="false">B10*$K$6</f>
+        <v>3.625</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>43504</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>24</v>
+      <c r="A11" s="6" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <f aca="false">B11*$K$6</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transaction view created, linked to from main
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">Before proceeding with views draw up wireframe using fixed model classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Layout, Main Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to ask about that auto complete html header thing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created structure ^ stitch in time. Content still basic.</t>
   </si>
 </sst>
 </file>
@@ -262,10 +271,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K12"/>
+  <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -275,7 +284,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
@@ -558,6 +567,9 @@
       <c r="A12" s="7" t="n">
         <v>43504</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C12" s="0" t="s">
         <v>20</v>
       </c>
@@ -569,6 +581,50 @@
       </c>
       <c r="F12" s="0" t="s">
         <v>35</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <f aca="false">B12*$K$6</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tag and merchant controllers created
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t xml:space="preserve">Created structure ^ stitch in time. Content still basic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Transaction Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements – don’t forget they’re up there and matter!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Merchant Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basically a copy of above, tested.</t>
   </si>
 </sst>
 </file>
@@ -271,10 +283,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K14"/>
+  <dimension ref="A2:K16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,6 +639,46 @@
         <v>38</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added Create new merchant functionality - tested with new transaction
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t xml:space="preserve">basically a copy of above, tested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Tag Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Transaction Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little bit of bother remembering which name points to the db</t>
   </si>
 </sst>
 </file>
@@ -283,10 +292,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K16"/>
+  <dimension ref="A2:K18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,6 +688,46 @@
         <v>42</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added get merchant index functionality to merchant view
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t xml:space="preserve">Little bit of bother remembering which name points to the db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Tag Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once you’ve done one…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Merchant Functionality</t>
   </si>
 </sst>
 </file>
@@ -292,10 +301,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K18"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -728,6 +737,46 @@
         <v>45</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="n">
+        <v>43504</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added merchant function for transaction model
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -167,6 +168,84 @@
   </si>
   <si>
     <t xml:space="preserve">Create Merchant Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create find merchant functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create find tag functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“And, baby, when I tell ya the boy has got his own money, I mean the boy has got his own MONEY!”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“I had the most absurd nightmare. I was poor and no one liked me.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Show me the MONEY!”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“There’s just one thing I want you to do for me Jerry...”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“I’m gonna teach you to hate spending money.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Look, money may be your god but it ain’t mine, alright? I want a warm bath and a cup of tea, over.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“What would you do if you had a million dollars...”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Napoleon, you know we can’t afford the fun pack. “</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Greed is good”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"That will be $1.5 million please. I’ll take it in cash, check or a transfer. I’m not greedy. I just want my half." </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"No dough, no show."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“There’s no nobility in poverty. I’ve been a poor man, and I’ve been a rich man. And I choose rich every f*cking time.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“I’m washing lettuce. Soon, I’ll be on fries. In a few years, I’ll make assistant manager, and that’s when the big bucks start rolling in.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“You fool! You’re 30 cents away from having a quarter!” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“A fool and his money are lucky enough to get together in the first place.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“The safest way to double your money is to fold it over and put it in your pocket.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Man, money ain't got no owners, only spenders”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Money be GREEN!”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“If you think nobody cares if you’re alive, try missing a couple of car payments.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Carpe per diem – seize the check.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“But you start to follow the money...”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"It takes money to make money, Stringer. Otherwise, hell, every pauper would be a king."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"All the pieces matter." </t>
+  </si>
+  <si>
+    <t xml:space="preserve">“It’s all in the game ...”</t>
   </si>
 </sst>
 </file>
@@ -251,7 +330,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,6 +363,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -301,10 +384,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -777,6 +860,40 @@
         <v>47</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -786,4 +903,153 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:B26"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="98.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="65.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="55.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="98.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="22.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="130.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="55.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="76.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit functionality added to transaction model
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t xml:space="preserve">Create find tag functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Transaction sum functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Edit Merchant functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nightmare owing to being unable to update unless all fields provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Edit Tag functionality</t>
   </si>
   <si>
     <t xml:space="preserve">“And, baby, when I tell ya the boy has got his own money, I mean the boy has got his own MONEY!”</t>
@@ -330,7 +342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +375,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -384,10 +400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K22"/>
+  <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,7 +412,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.23"/>
@@ -892,6 +908,83 @@
       </c>
       <c r="E22" s="0" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -912,8 +1005,8 @@
   </sheetPr>
   <dimension ref="B3:B26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -924,123 +1017,123 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="98.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="s">
-        <v>51</v>
+      <c r="B3" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="65.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
-        <v>52</v>
+      <c r="B4" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="55.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
-        <v>55</v>
+      <c r="B7" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
-        <v>56</v>
+      <c r="B8" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
-        <v>58</v>
+      <c r="B10" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="98.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
-        <v>60</v>
+      <c r="B12" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8" t="s">
-        <v>61</v>
+      <c r="B13" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8" t="s">
-        <v>62</v>
+      <c r="B14" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="130.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8" t="s">
-        <v>63</v>
+      <c r="B15" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="55.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8" t="s">
-        <v>64</v>
+      <c r="B16" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="76.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8" t="s">
-        <v>65</v>
+      <c r="B17" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8" t="s">
-        <v>69</v>
+      <c r="B21" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cycle 1 reflection, Cycle 2 planning
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -173,6 +173,9 @@
     <t xml:space="preserve">Create find merchant functionality</t>
   </si>
   <si>
+    <t xml:space="preserve">Straight forward after doing so much of it</t>
+  </si>
+  <si>
     <t xml:space="preserve">Create find tag functionality</t>
   </si>
   <si>
@@ -186,6 +189,30 @@
   </si>
   <si>
     <t xml:space="preserve">Create Edit Tag functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once you’ve done one…plus bonus dynamic selectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bugfix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction.amount_int to float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well. This is embarrassing. D*ck. Monetary values should be float. Ground up howler.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction total truncating trailing zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed by converting to string using 2f string formatting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discover user needs and measure against time remaining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have to be careful, play it safe – leave Tue/Wed for CSS malark.</t>
   </si>
   <si>
     <t xml:space="preserve">“And, baby, when I tell ya the boy has got his own money, I mean the boy has got his own MONEY!”</t>
@@ -400,10 +427,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K26"/>
+  <dimension ref="A2:K29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -892,6 +919,9 @@
       <c r="E21" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="F21" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="n">
@@ -907,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,10 +971,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>47</v>
@@ -972,7 +1002,7 @@
         <v>43505</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>26</v>
@@ -981,10 +1011,67 @@
         <v>1</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
+        <v>43505</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1006,7 +1093,7 @@
   <dimension ref="B3:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="1" sqref="B7:B20 B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1018,122 +1105,122 @@
   <sheetData>
     <row r="3" customFormat="false" ht="98.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="9" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="65.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="55.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="87.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="98.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="9" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="44.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="130.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="55.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="9" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="76.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added show transactions for tag and sum functionality to tag model
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -233,6 +233,21 @@
   </si>
   <si>
     <t xml:space="preserve">What needs done in which order. Dates. Just dates. Fuck.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove unecessary ID columns from view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simple enough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add transactions view to merchant model and sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum was a waste as I forgot to access PG object using string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add transactions view to tag model and sum</t>
   </si>
 </sst>
 </file>
@@ -317,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -346,6 +361,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -363,10 +382,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K32"/>
+  <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1163,6 +1182,68 @@
         <v>58</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="n">
+        <v>43507</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
+        <v>43507</v>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated tag db schema,specs,model & views to include budget
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add transactions view to tag model and sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once you’ve done one…then you spot bugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add budget to tags table, controller, specs and views</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K35"/>
+  <dimension ref="A2:K43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1229,7 +1235,7 @@
         <v>43507</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>26</v>
@@ -1241,7 +1247,98 @@
         <v>75</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>47</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date to transaction db schema, model,view and controller
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add budget to tags table, controller, specs and views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Straightforward – planning really helped with this one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add date to transactions table, controller, specs and views</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
   <dimension ref="A2:K43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1254,6 +1260,9 @@
       <c r="A36" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B36" s="0" t="n">
+        <v>0.75</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>26</v>
       </c>
@@ -1262,6 +1271,9 @@
       </c>
       <c r="E36" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,6 +1285,9 @@
       </c>
       <c r="D37" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added sorting facilities to transaction MVC
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -260,6 +260,33 @@
   </si>
   <si>
     <t xml:space="preserve">Add date to transactions table, controller, specs and views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">straightforward enough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create struct to hold budget in tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">should have continued with this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display total amount spent per tag per month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR not due to struct but using post rather than get</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rebuild a budget class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feels a bit surplus and details not persisted? Would have liked the struct route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show totals for month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">straight forward enough</t>
   </si>
 </sst>
 </file>
@@ -396,8 +423,8 @@
   </sheetPr>
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1280,6 +1307,9 @@
       <c r="A37" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>26</v>
       </c>
@@ -1288,50 +1318,89 @@
       </c>
       <c r="E37" s="0" t="s">
         <v>79</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added sort function to Merchant MVC
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -287,6 +287,18 @@
   </si>
   <si>
     <t xml:space="preserve">straight forward enough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create warning/over identifiers for budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Sort Function for Transaction class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL was not happy with this at all – would not accept params no matter what I did</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Sort Function for Tag Class</t>
   </si>
 </sst>
 </file>
@@ -421,10 +433,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K43"/>
+  <dimension ref="A2:K44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -638,8 +650,8 @@
         <v>25</v>
       </c>
       <c r="K8" s="0" t="n">
-        <f aca="false">SUM(B3:B32)</f>
-        <v>33.25</v>
+        <f aca="false">SUM(B3:B100)</f>
+        <v>44.75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +682,7 @@
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K6*K8</f>
-        <v>482.125</v>
+        <v>648.875</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,7 +1252,10 @@
       <c r="F33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="5" t="n">
+        <f aca="false">B33*$K$6</f>
+        <v>7.25</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
@@ -1261,7 +1276,10 @@
       <c r="F34" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="5" t="n">
+        <f aca="false">B34*$K$6</f>
+        <v>14.5</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="n">
@@ -1282,6 +1300,10 @@
       <c r="F35" s="0" t="s">
         <v>76</v>
       </c>
+      <c r="G35" s="5" t="n">
+        <f aca="false">B35*$K$6</f>
+        <v>7.25</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="n">
@@ -1302,6 +1324,10 @@
       <c r="F36" s="0" t="s">
         <v>78</v>
       </c>
+      <c r="G36" s="5" t="n">
+        <f aca="false">B36*$K$6</f>
+        <v>10.875</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="n">
@@ -1322,6 +1348,10 @@
       <c r="F37" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="G37" s="5" t="n">
+        <f aca="false">B37*$K$6</f>
+        <v>14.5</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="n">
@@ -1342,6 +1372,10 @@
       <c r="F38" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="G38" s="5" t="n">
+        <f aca="false">B38*$K$6</f>
+        <v>14.5</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="n">
@@ -1362,6 +1396,10 @@
       <c r="F39" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="G39" s="5" t="n">
+        <f aca="false">B39*$K$6</f>
+        <v>14.5</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="n">
@@ -1382,6 +1420,10 @@
       <c r="F40" s="0" t="s">
         <v>86</v>
       </c>
+      <c r="G40" s="5" t="n">
+        <f aca="false">B40*$K$6</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="n">
@@ -1402,27 +1444,78 @@
       <c r="F41" s="0" t="s">
         <v>88</v>
       </c>
+      <c r="G41" s="5" t="n">
+        <f aca="false">B41*$K$6</f>
+        <v>14.5</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B42" s="0" t="n">
+        <v>0.5</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="5" t="n">
+        <f aca="false">B42*$K$6</f>
+        <v>7.25</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="n">
         <v>43507</v>
       </c>
+      <c r="B43" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" s="5" t="n">
+        <f aca="false">B43*$K$6</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="5" t="n">
+        <f aca="false">B44*$K$6</f>
+        <v>3.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged budgets views, reflected in controller
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">Discover user needs and measure against time remaining</t>
   </si>
   <si>
-    <t xml:space="preserve">Have to be careful, play it safe – leave Tue/Wed for CSS malark.</t>
+    <t xml:space="preserve">Have to be careful, play it safe – leave Tue/Wed for CSS malarky.</t>
   </si>
   <si>
     <t xml:space="preserve">How can you go about meeting above?</t>
@@ -292,6 +292,9 @@
     <t xml:space="preserve">Create warning/over identifiers for budget</t>
   </si>
   <si>
+    <t xml:space="preserve">Replace with images later</t>
+  </si>
+  <si>
     <t xml:space="preserve">Create Sort Function for Transaction class</t>
   </si>
   <si>
@@ -299,6 +302,18 @@
   </si>
   <si>
     <t xml:space="preserve">Create Sort Function for Tag Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Sort Function for Merchant Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arguably pointless, done fo consistency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge budget views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No need to have two separate pages if get used creatively</t>
   </si>
 </sst>
 </file>
@@ -433,10 +448,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K44"/>
+  <dimension ref="A2:K46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -650,8 +665,8 @@
         <v>25</v>
       </c>
       <c r="K8" s="0" t="n">
-        <f aca="false">SUM(B3:B100)</f>
-        <v>44.75</v>
+        <f aca="false">SUM(B3:B101)</f>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,7 +697,7 @@
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K6*K8</f>
-        <v>648.875</v>
+        <v>652.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,6 +1480,9 @@
       <c r="E42" s="0" t="s">
         <v>89</v>
       </c>
+      <c r="F42" s="0" t="s">
+        <v>90</v>
+      </c>
       <c r="G42" s="5" t="n">
         <f aca="false">B42*$K$6</f>
         <v>7.25</v>
@@ -1484,10 +1502,10 @@
         <v>2</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G43" s="5" t="n">
         <f aca="false">B43*$K$6</f>
@@ -1508,7 +1526,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>47</v>
@@ -1516,6 +1534,44 @@
       <c r="G44" s="5" t="n">
         <f aca="false">B44*$K$6</f>
         <v>3.625</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="n">
+        <v>43507</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="n">
+        <v>43508</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfix: Partial csv code implemented in budgets view removed. Phase 2 reflection
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -295,16 +295,16 @@
     <t xml:space="preserve">Replace with images later</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Sort Function for Transaction class</t>
+    <t xml:space="preserve">Create Sort Function for Transaction Controller</t>
   </si>
   <si>
     <t xml:space="preserve">SQL was not happy with this at all – would not accept params no matter what I did</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Sort Function for Tag Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Sort Function for Merchant Class</t>
+    <t xml:space="preserve">Create Sort Function for Tag Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Sort Function for Merchant Controller</t>
   </si>
   <si>
     <t xml:space="preserve">Arguably pointless, done fo consistency</t>
@@ -314,6 +314,18 @@
   </si>
   <si>
     <t xml:space="preserve">No need to have two separate pages if get used creatively</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Sort Function for Budget Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once you’ve done one...are sorts always in controller?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review views for phase 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put CSV import/export on hold until CSS done, product is stable.</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K46"/>
+  <dimension ref="A2:K48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -666,7 +678,7 @@
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">SUM(B3:B101)</f>
-        <v>45</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,7 +709,7 @@
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K6*K8</f>
-        <v>652.5</v>
+        <v>674.25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,7 +1573,10 @@
       <c r="A46" s="7" t="n">
         <v>43508</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="B46" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="0" t="n">
@@ -1572,6 +1587,46 @@
       </c>
       <c r="F46" s="0" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="n">
+        <v>43508</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="n">
+        <v>43508</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tag transaction table
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t xml:space="preserve">Put CSV import/export on hold until CSS done, product is stable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">understanding/Styling Home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battering my heid against a wall trying to comprehend CSS and how it relates to this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styling Tables/Icons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting a bit more confident – afraid to do the layout and break it all</t>
   </si>
 </sst>
 </file>
@@ -460,10 +475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K48"/>
+  <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -678,7 +693,7 @@
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">SUM(B3:B101)</f>
-        <v>46.5</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +724,7 @@
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K6*K8</f>
-        <v>674.25</v>
+        <v>790.25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1582,10 @@
       <c r="F45" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="n">
+        <f aca="false">B45*$K$6</f>
+        <v>3.625</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="n">
@@ -1588,6 +1606,10 @@
       <c r="F46" s="0" t="s">
         <v>97</v>
       </c>
+      <c r="G46" s="5" t="n">
+        <f aca="false">B46*$K$6</f>
+        <v>7.25</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="n">
@@ -1608,6 +1630,10 @@
       <c r="F47" s="0" t="s">
         <v>99</v>
       </c>
+      <c r="G47" s="5" t="n">
+        <f aca="false">B47*$K$6</f>
+        <v>7.25</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="n">
@@ -1627,6 +1653,58 @@
       </c>
       <c r="F48" s="0" t="s">
         <v>101</v>
+      </c>
+      <c r="G48" s="5" t="n">
+        <f aca="false">B48*$K$6</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="n">
+        <v>43508</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" s="5" t="n">
+        <f aca="false">B49*$K$6</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7" t="n">
+        <v>43508</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G50" s="5" t="n">
+        <f aca="false">B50*$K$6</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added icons to header, added £ to merchant transactions
</commit_message>
<xml_diff>
--- a/FEED/Reporting.xlsx
+++ b/FEED/Reporting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">Styling</t>
   </si>
   <si>
-    <t xml:space="preserve">understanding/Styling Home page</t>
+    <t xml:space="preserve">Understanding/Styling Home page</t>
   </si>
   <si>
     <t xml:space="preserve">Battering my heid against a wall trying to comprehend CSS and how it relates to this</t>
@@ -475,10 +475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K50"/>
+  <dimension ref="A2:K51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="50:50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,7 +693,7 @@
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">SUM(B3:B101)</f>
-        <v>54.5</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +724,7 @@
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">K6*K8</f>
-        <v>790.25</v>
+        <v>819.25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,6 +1705,26 @@
       <c r="G50" s="5" t="n">
         <f aca="false">B50*$K$6</f>
         <v>29</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="n">
+        <v>43508</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>